<commit_message>
Add: jumlah_muatan_usaha_wilkerstat colomn in daftar-desa.xlsx
</commit_message>
<xml_diff>
--- a/public/daftar-desa.xlsx
+++ b/public/daftar-desa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\magang bps nganjuk\geotagging kendedes\desa-tagging-dashboard\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{870BA1E4-37A4-4DF9-B8DC-80711D6C0E55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7F5FD5-FEAB-4031-B6E4-929223C13EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7EE119A2-899B-4DBB-B915-ACB8547C4074}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="280">
   <si>
     <t>SAWAHAN</t>
   </si>
@@ -871,6 +871,9 @@
   </si>
   <si>
     <t>desa</t>
+  </si>
+  <si>
+    <t>jumlah_muatan_usaha_wilkerstat</t>
   </si>
 </sst>
 </file>
@@ -928,12 +931,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1250,10 +1256,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7F1BDDB-B22A-4172-A0C6-319A22332B75}">
-  <dimension ref="A1:C285"/>
+  <dimension ref="A1:D285"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1261,9 +1267,10 @@
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>276</v>
       </c>
@@ -1273,8 +1280,11 @@
       <c r="C1" s="2" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>3518010001</v>
       </c>
@@ -1284,8 +1294,11 @@
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" s="1">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>3518010002</v>
       </c>
@@ -1295,8 +1308,11 @@
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="1">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3518010003</v>
       </c>
@@ -1306,8 +1322,11 @@
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" s="1">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3518010004</v>
       </c>
@@ -1317,8 +1336,11 @@
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" s="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>3518010005</v>
       </c>
@@ -1328,8 +1350,11 @@
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" s="1">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>3518010006</v>
       </c>
@@ -1339,8 +1364,11 @@
       <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" s="1">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>3518010007</v>
       </c>
@@ -1350,8 +1378,11 @@
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" s="1">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>3518010008</v>
       </c>
@@ -1361,8 +1392,11 @@
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" s="1">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>3518010009</v>
       </c>
@@ -1372,8 +1406,11 @@
       <c r="C10" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" s="1">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>3518020001</v>
       </c>
@@ -1383,8 +1420,11 @@
       <c r="C11" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>3518020002</v>
       </c>
@@ -1394,8 +1434,11 @@
       <c r="C12" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" s="1">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>3518020003</v>
       </c>
@@ -1405,8 +1448,11 @@
       <c r="C13" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13" s="1">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>3518020004</v>
       </c>
@@ -1416,8 +1462,11 @@
       <c r="C14" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14" s="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>3518020005</v>
       </c>
@@ -1427,8 +1476,11 @@
       <c r="C15" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15" s="1">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>3518020006</v>
       </c>
@@ -1438,8 +1490,11 @@
       <c r="C16" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16" s="1">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>3518020007</v>
       </c>
@@ -1449,8 +1504,11 @@
       <c r="C17" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17" s="1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>3518020008</v>
       </c>
@@ -1460,8 +1518,11 @@
       <c r="C18" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18" s="1">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>3518020009</v>
       </c>
@@ -1471,8 +1532,11 @@
       <c r="C19" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19" s="1">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>3518030001</v>
       </c>
@@ -1482,8 +1546,11 @@
       <c r="C20" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20" s="1">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>3518030002</v>
       </c>
@@ -1493,8 +1560,11 @@
       <c r="C21" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21" s="1">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>3518030003</v>
       </c>
@@ -1504,8 +1574,11 @@
       <c r="C22" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D22" s="1">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>3518030004</v>
       </c>
@@ -1515,8 +1588,11 @@
       <c r="C23" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D23" s="1">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>3518030005</v>
       </c>
@@ -1526,8 +1602,11 @@
       <c r="C24" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24" s="1">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>3518030006</v>
       </c>
@@ -1537,8 +1616,11 @@
       <c r="C25" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D25" s="1">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>3518030007</v>
       </c>
@@ -1548,8 +1630,11 @@
       <c r="C26" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26" s="1">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>3518030008</v>
       </c>
@@ -1559,8 +1644,11 @@
       <c r="C27" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D27" s="1">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>3518030009</v>
       </c>
@@ -1570,8 +1658,11 @@
       <c r="C28" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D28" s="1">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>3518030010</v>
       </c>
@@ -1581,8 +1672,11 @@
       <c r="C29" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D29" s="1">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>3518030011</v>
       </c>
@@ -1592,8 +1686,11 @@
       <c r="C30" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D30" s="1">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>3518030012</v>
       </c>
@@ -1603,8 +1700,11 @@
       <c r="C31" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D31" s="1">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>3518030013</v>
       </c>
@@ -1614,8 +1714,11 @@
       <c r="C32" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D32" s="1">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>3518030014</v>
       </c>
@@ -1625,8 +1728,11 @@
       <c r="C33" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D33" s="1">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>3518030015</v>
       </c>
@@ -1636,8 +1742,11 @@
       <c r="C34" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D34" s="1">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>3518030016</v>
       </c>
@@ -1647,8 +1756,11 @@
       <c r="C35" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D35" s="1">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>3518030017</v>
       </c>
@@ -1658,8 +1770,11 @@
       <c r="C36" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D36" s="1">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>3518030018</v>
       </c>
@@ -1669,8 +1784,11 @@
       <c r="C37" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D37" s="1">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>3518030019</v>
       </c>
@@ -1680,8 +1798,11 @@
       <c r="C38" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D38" s="1">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>3518040001</v>
       </c>
@@ -1691,8 +1812,11 @@
       <c r="C39" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D39" s="1">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>3518040002</v>
       </c>
@@ -1702,8 +1826,11 @@
       <c r="C40" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D40" s="1">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>3518040003</v>
       </c>
@@ -1713,8 +1840,11 @@
       <c r="C41" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D41" s="1">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>3518040004</v>
       </c>
@@ -1724,8 +1854,11 @@
       <c r="C42" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D42" s="1">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>3518040005</v>
       </c>
@@ -1735,8 +1868,11 @@
       <c r="C43" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D43" s="1">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>3518040006</v>
       </c>
@@ -1746,8 +1882,11 @@
       <c r="C44" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D44" s="1">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>3518040007</v>
       </c>
@@ -1757,8 +1896,11 @@
       <c r="C45" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D45" s="1">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>3518040008</v>
       </c>
@@ -1768,8 +1910,11 @@
       <c r="C46" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D46" s="1">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>3518040009</v>
       </c>
@@ -1779,8 +1924,11 @@
       <c r="C47" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D47" s="1">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>3518040010</v>
       </c>
@@ -1790,8 +1938,11 @@
       <c r="C48" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D48" s="1">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>3518040011</v>
       </c>
@@ -1801,8 +1952,11 @@
       <c r="C49" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D49" s="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>3518040012</v>
       </c>
@@ -1812,8 +1966,11 @@
       <c r="C50" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D50" s="1">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>3518040013</v>
       </c>
@@ -1823,8 +1980,11 @@
       <c r="C51" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D51" s="1">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>3518040014</v>
       </c>
@@ -1834,8 +1994,11 @@
       <c r="C52" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D52" s="1">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>3518040015</v>
       </c>
@@ -1845,8 +2008,11 @@
       <c r="C53" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D53" s="1">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>3518040016</v>
       </c>
@@ -1856,8 +2022,11 @@
       <c r="C54" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D54" s="1">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>3518040017</v>
       </c>
@@ -1867,8 +2036,11 @@
       <c r="C55" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D55" s="1">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>3518040018</v>
       </c>
@@ -1878,8 +2050,11 @@
       <c r="C56" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D56" s="1">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>3518040019</v>
       </c>
@@ -1889,8 +2064,11 @@
       <c r="C57" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D57" s="1">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>3518040020</v>
       </c>
@@ -1900,8 +2078,11 @@
       <c r="C58" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D58" s="1">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>3518040021</v>
       </c>
@@ -1911,8 +2092,11 @@
       <c r="C59" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D59" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>3518040022</v>
       </c>
@@ -1922,8 +2106,11 @@
       <c r="C60" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D60" s="1">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>3518050001</v>
       </c>
@@ -1933,8 +2120,11 @@
       <c r="C61" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D61" s="1">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>3518050002</v>
       </c>
@@ -1944,8 +2134,11 @@
       <c r="C62" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D62" s="1">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>3518050003</v>
       </c>
@@ -1955,8 +2148,11 @@
       <c r="C63" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D63" s="1">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>3518050004</v>
       </c>
@@ -1966,8 +2162,11 @@
       <c r="C64" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D64" s="1">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>3518050005</v>
       </c>
@@ -1977,8 +2176,11 @@
       <c r="C65" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D65" s="1">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>3518050006</v>
       </c>
@@ -1988,8 +2190,11 @@
       <c r="C66" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D66" s="1">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>3518050007</v>
       </c>
@@ -1999,8 +2204,11 @@
       <c r="C67" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D67" s="1">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>3518050008</v>
       </c>
@@ -2010,8 +2218,11 @@
       <c r="C68" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D68" s="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>3518050009</v>
       </c>
@@ -2021,8 +2232,11 @@
       <c r="C69" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D69" s="1">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>3518050010</v>
       </c>
@@ -2032,8 +2246,11 @@
       <c r="C70" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D70" s="1">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>3518050011</v>
       </c>
@@ -2043,8 +2260,11 @@
       <c r="C71" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D71" s="1">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>3518050012</v>
       </c>
@@ -2054,8 +2274,11 @@
       <c r="C72" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D72" s="1">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>3518050013</v>
       </c>
@@ -2065,8 +2288,11 @@
       <c r="C73" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D73" s="1">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>3518050014</v>
       </c>
@@ -2076,8 +2302,11 @@
       <c r="C74" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D74" s="1">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>3518050015</v>
       </c>
@@ -2087,8 +2316,11 @@
       <c r="C75" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D75" s="1">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>3518050016</v>
       </c>
@@ -2098,8 +2330,11 @@
       <c r="C76" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D76" s="1">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>3518050017</v>
       </c>
@@ -2109,8 +2344,11 @@
       <c r="C77" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D77" s="1">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>3518050018</v>
       </c>
@@ -2120,8 +2358,11 @@
       <c r="C78" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D78" s="1">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>3518060001</v>
       </c>
@@ -2131,8 +2372,11 @@
       <c r="C79" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D79" s="1">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>3518060002</v>
       </c>
@@ -2142,8 +2386,11 @@
       <c r="C80" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D80" s="1">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>3518060004</v>
       </c>
@@ -2153,8 +2400,11 @@
       <c r="C81" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D81" s="1">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>3518060005</v>
       </c>
@@ -2164,8 +2414,11 @@
       <c r="C82" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D82" s="1">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>3518060006</v>
       </c>
@@ -2175,8 +2428,11 @@
       <c r="C83" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D83" s="1">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>3518060007</v>
       </c>
@@ -2186,8 +2442,11 @@
       <c r="C84" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D84" s="1">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>3518060008</v>
       </c>
@@ -2197,8 +2456,11 @@
       <c r="C85" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D85" s="1">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>3518060009</v>
       </c>
@@ -2208,8 +2470,11 @@
       <c r="C86" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D86" s="1">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>3518060010</v>
       </c>
@@ -2219,8 +2484,11 @@
       <c r="C87" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D87" s="1">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>3518060012</v>
       </c>
@@ -2230,8 +2498,11 @@
       <c r="C88" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D88" s="1">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>3518060013</v>
       </c>
@@ -2241,8 +2512,11 @@
       <c r="C89" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D89" s="1">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>3518060014</v>
       </c>
@@ -2252,8 +2526,11 @@
       <c r="C90" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D90" s="1">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>3518060015</v>
       </c>
@@ -2263,8 +2540,11 @@
       <c r="C91" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D91" s="1">
+        <v>2845</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>3518060016</v>
       </c>
@@ -2274,8 +2554,11 @@
       <c r="C92" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D92" s="1">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>3518060018</v>
       </c>
@@ -2285,8 +2568,11 @@
       <c r="C93" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D93" s="1">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>3518060019</v>
       </c>
@@ -2296,8 +2582,11 @@
       <c r="C94" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D94" s="1">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>3518070001</v>
       </c>
@@ -2307,8 +2596,11 @@
       <c r="C95" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D95" s="1">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>3518070002</v>
       </c>
@@ -2318,8 +2610,11 @@
       <c r="C96" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D96" s="1">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>3518070003</v>
       </c>
@@ -2329,8 +2624,11 @@
       <c r="C97" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D97" s="1">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>3518070004</v>
       </c>
@@ -2340,8 +2638,11 @@
       <c r="C98" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D98" s="1">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>3518070005</v>
       </c>
@@ -2351,8 +2652,11 @@
       <c r="C99" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D99" s="1">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>3518070006</v>
       </c>
@@ -2362,8 +2666,11 @@
       <c r="C100" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D100" s="1">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>3518070007</v>
       </c>
@@ -2373,8 +2680,11 @@
       <c r="C101" s="1" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D101" s="1">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>3518070008</v>
       </c>
@@ -2384,8 +2694,11 @@
       <c r="C102" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D102" s="1">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>3518070009</v>
       </c>
@@ -2395,8 +2708,11 @@
       <c r="C103" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D103" s="1">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>3518070010</v>
       </c>
@@ -2406,8 +2722,11 @@
       <c r="C104" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D104" s="1">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>3518070011</v>
       </c>
@@ -2417,8 +2736,11 @@
       <c r="C105" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D105" s="1">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>3518070012</v>
       </c>
@@ -2428,8 +2750,11 @@
       <c r="C106" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D106" s="1">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>3518070013</v>
       </c>
@@ -2439,8 +2764,11 @@
       <c r="C107" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D107" s="1">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>3518070014</v>
       </c>
@@ -2450,8 +2778,11 @@
       <c r="C108" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D108" s="1">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>3518080001</v>
       </c>
@@ -2461,8 +2792,11 @@
       <c r="C109" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D109" s="1">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>3518080002</v>
       </c>
@@ -2472,8 +2806,11 @@
       <c r="C110" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D110" s="1">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>3518080003</v>
       </c>
@@ -2483,8 +2820,11 @@
       <c r="C111" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D111" s="1">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>3518080004</v>
       </c>
@@ -2494,8 +2834,11 @@
       <c r="C112" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D112" s="1">
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>3518080005</v>
       </c>
@@ -2505,8 +2848,11 @@
       <c r="C113" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D113" s="1">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>3518080006</v>
       </c>
@@ -2516,8 +2862,11 @@
       <c r="C114" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D114" s="1">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>3518080007</v>
       </c>
@@ -2527,8 +2876,11 @@
       <c r="C115" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D115" s="1">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>3518080008</v>
       </c>
@@ -2538,8 +2890,11 @@
       <c r="C116" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D116" s="1">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>3518080009</v>
       </c>
@@ -2549,8 +2904,11 @@
       <c r="C117" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D117" s="1">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>3518080010</v>
       </c>
@@ -2560,8 +2918,11 @@
       <c r="C118" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D118" s="1">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>3518080011</v>
       </c>
@@ -2571,8 +2932,11 @@
       <c r="C119" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D119" s="1">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>3518080012</v>
       </c>
@@ -2582,8 +2946,11 @@
       <c r="C120" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D120" s="1">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>3518080013</v>
       </c>
@@ -2593,8 +2960,11 @@
       <c r="C121" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D121" s="1">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>3518090001</v>
       </c>
@@ -2604,8 +2974,11 @@
       <c r="C122" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D122" s="1">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>3518090002</v>
       </c>
@@ -2615,8 +2988,11 @@
       <c r="C123" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D123" s="1">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>3518090003</v>
       </c>
@@ -2626,8 +3002,11 @@
       <c r="C124" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D124" s="1">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>3518090004</v>
       </c>
@@ -2637,8 +3016,11 @@
       <c r="C125" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D125" s="1">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>3518090005</v>
       </c>
@@ -2648,8 +3030,11 @@
       <c r="C126" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D126" s="1">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>3518090006</v>
       </c>
@@ -2659,8 +3044,11 @@
       <c r="C127" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D127" s="1">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>3518090007</v>
       </c>
@@ -2670,8 +3058,11 @@
       <c r="C128" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D128" s="1">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>3518090008</v>
       </c>
@@ -2681,8 +3072,11 @@
       <c r="C129" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D129" s="1">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>3518090009</v>
       </c>
@@ -2692,8 +3086,11 @@
       <c r="C130" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D130" s="1">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>3518090010</v>
       </c>
@@ -2703,8 +3100,11 @@
       <c r="C131" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D131" s="1">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>3518090011</v>
       </c>
@@ -2714,8 +3114,11 @@
       <c r="C132" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D132" s="1">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>3518090012</v>
       </c>
@@ -2725,8 +3128,11 @@
       <c r="C133" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D133" s="1">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>3518090013</v>
       </c>
@@ -2736,8 +3142,11 @@
       <c r="C134" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D134" s="1">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>3518090014</v>
       </c>
@@ -2747,8 +3156,11 @@
       <c r="C135" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D135" s="1">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>3518100001</v>
       </c>
@@ -2758,8 +3170,11 @@
       <c r="C136" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D136" s="1">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>3518100002</v>
       </c>
@@ -2769,8 +3184,11 @@
       <c r="C137" s="1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D137" s="1">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>3518100003</v>
       </c>
@@ -2780,8 +3198,11 @@
       <c r="C138" s="1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D138" s="1">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>3518100004</v>
       </c>
@@ -2791,8 +3212,11 @@
       <c r="C139" s="1" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D139" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>3518100005</v>
       </c>
@@ -2802,8 +3226,11 @@
       <c r="C140" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D140" s="1">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>3518100006</v>
       </c>
@@ -2813,8 +3240,11 @@
       <c r="C141" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D141" s="1">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>3518100007</v>
       </c>
@@ -2824,8 +3254,11 @@
       <c r="C142" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D142" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>3518100008</v>
       </c>
@@ -2835,8 +3268,11 @@
       <c r="C143" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D143" s="1">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>3518100009</v>
       </c>
@@ -2846,8 +3282,11 @@
       <c r="C144" s="1" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D144" s="1">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <v>3518100010</v>
       </c>
@@ -2857,8 +3296,11 @@
       <c r="C145" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D145" s="1">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <v>3518100011</v>
       </c>
@@ -2868,8 +3310,11 @@
       <c r="C146" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D146" s="1">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
         <v>3518110001</v>
       </c>
@@ -2879,8 +3324,11 @@
       <c r="C147" s="1" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D147" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <v>3518110002</v>
       </c>
@@ -2890,8 +3338,11 @@
       <c r="C148" s="1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D148" s="1">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>3518110003</v>
       </c>
@@ -2901,8 +3352,11 @@
       <c r="C149" s="1" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D149" s="1">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" s="1">
         <v>3518110004</v>
       </c>
@@ -2912,8 +3366,11 @@
       <c r="C150" s="1" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D150" s="1">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" s="1">
         <v>3518110005</v>
       </c>
@@ -2923,8 +3380,11 @@
       <c r="C151" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D151" s="1">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" s="1">
         <v>3518110006</v>
       </c>
@@ -2934,8 +3394,11 @@
       <c r="C152" s="1" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D152" s="1">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" s="1">
         <v>3518110007</v>
       </c>
@@ -2945,8 +3408,11 @@
       <c r="C153" s="1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D153" s="1">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" s="1">
         <v>3518110008</v>
       </c>
@@ -2956,8 +3422,11 @@
       <c r="C154" s="1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D154" s="1">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" s="1">
         <v>3518110009</v>
       </c>
@@ -2967,8 +3436,11 @@
       <c r="C155" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D155" s="1">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" s="1">
         <v>3518110010</v>
       </c>
@@ -2978,8 +3450,11 @@
       <c r="C156" s="1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D156" s="1">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" s="1">
         <v>3518110011</v>
       </c>
@@ -2989,8 +3464,11 @@
       <c r="C157" s="1" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D157" s="1">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" s="1">
         <v>3518120001</v>
       </c>
@@ -3000,8 +3478,11 @@
       <c r="C158" s="1" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D158" s="1">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" s="1">
         <v>3518120002</v>
       </c>
@@ -3011,8 +3492,11 @@
       <c r="C159" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D159" s="1">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" s="1">
         <v>3518120003</v>
       </c>
@@ -3022,8 +3506,11 @@
       <c r="C160" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D160" s="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" s="1">
         <v>3518120004</v>
       </c>
@@ -3033,8 +3520,11 @@
       <c r="C161" s="1" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D161" s="1">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" s="1">
         <v>3518120005</v>
       </c>
@@ -3044,8 +3534,11 @@
       <c r="C162" s="1" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D162" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" s="1">
         <v>3518120006</v>
       </c>
@@ -3055,8 +3548,11 @@
       <c r="C163" s="1" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D163" s="1">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" s="1">
         <v>3518120007</v>
       </c>
@@ -3066,8 +3562,11 @@
       <c r="C164" s="1" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D164" s="1">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" s="1">
         <v>3518120008</v>
       </c>
@@ -3077,8 +3576,11 @@
       <c r="C165" s="1" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D165" s="1">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" s="1">
         <v>3518120009</v>
       </c>
@@ -3088,8 +3590,11 @@
       <c r="C166" s="1" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D166" s="1">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" s="1">
         <v>3518120010</v>
       </c>
@@ -3099,8 +3604,11 @@
       <c r="C167" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D167" s="1">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" s="1">
         <v>3518120011</v>
       </c>
@@ -3110,8 +3618,11 @@
       <c r="C168" s="1" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D168" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" s="1">
         <v>3518120012</v>
       </c>
@@ -3121,8 +3632,11 @@
       <c r="C169" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D169" s="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" s="1">
         <v>3518120013</v>
       </c>
@@ -3132,8 +3646,11 @@
       <c r="C170" s="1" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D170" s="1">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" s="1">
         <v>3518120014</v>
       </c>
@@ -3143,8 +3660,11 @@
       <c r="C171" s="1" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D171" s="1">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" s="1">
         <v>3518120015</v>
       </c>
@@ -3154,8 +3674,11 @@
       <c r="C172" s="1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D172" s="1">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" s="1">
         <v>3518120016</v>
       </c>
@@ -3165,8 +3688,11 @@
       <c r="C173" s="1" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D173" s="1">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" s="1">
         <v>3518120017</v>
       </c>
@@ -3176,8 +3702,11 @@
       <c r="C174" s="1" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D174" s="1">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" s="1">
         <v>3518130001</v>
       </c>
@@ -3187,8 +3716,11 @@
       <c r="C175" s="1" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D175" s="1">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" s="1">
         <v>3518130002</v>
       </c>
@@ -3198,8 +3730,11 @@
       <c r="C176" s="1" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D176" s="1">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" s="1">
         <v>3518130003</v>
       </c>
@@ -3209,8 +3744,11 @@
       <c r="C177" s="1" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D177" s="1">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" s="1">
         <v>3518130004</v>
       </c>
@@ -3220,8 +3758,11 @@
       <c r="C178" s="1" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D178" s="1">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" s="1">
         <v>3518130005</v>
       </c>
@@ -3231,8 +3772,11 @@
       <c r="C179" s="1" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D179" s="1">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" s="1">
         <v>3518130006</v>
       </c>
@@ -3242,8 +3786,11 @@
       <c r="C180" s="1" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D180" s="1">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" s="1">
         <v>3518130007</v>
       </c>
@@ -3253,8 +3800,11 @@
       <c r="C181" s="1" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D181" s="1">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" s="1">
         <v>3518130008</v>
       </c>
@@ -3264,8 +3814,11 @@
       <c r="C182" s="1" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D182" s="1">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" s="1">
         <v>3518130009</v>
       </c>
@@ -3275,8 +3828,11 @@
       <c r="C183" s="1" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D183" s="1">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" s="1">
         <v>3518130010</v>
       </c>
@@ -3286,8 +3842,11 @@
       <c r="C184" s="1" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D184" s="1">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" s="1">
         <v>3518130011</v>
       </c>
@@ -3297,8 +3856,11 @@
       <c r="C185" s="1" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D185" s="1">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" s="1">
         <v>3518130012</v>
       </c>
@@ -3308,8 +3870,11 @@
       <c r="C186" s="1" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D186" s="1">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" s="1">
         <v>3518140001</v>
       </c>
@@ -3319,8 +3884,11 @@
       <c r="C187" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D187" s="1">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" s="1">
         <v>3518140002</v>
       </c>
@@ -3330,8 +3898,11 @@
       <c r="C188" s="1" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D188" s="1">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" s="1">
         <v>3518140003</v>
       </c>
@@ -3341,8 +3912,11 @@
       <c r="C189" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D189" s="1">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" s="1">
         <v>3518140004</v>
       </c>
@@ -3352,8 +3926,11 @@
       <c r="C190" s="1" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D190" s="1">
+        <v>1895</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" s="1">
         <v>3518140005</v>
       </c>
@@ -3363,8 +3940,11 @@
       <c r="C191" s="1" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D191" s="1">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" s="1">
         <v>3518140006</v>
       </c>
@@ -3374,8 +3954,11 @@
       <c r="C192" s="1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D192" s="1">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" s="1">
         <v>3518140007</v>
       </c>
@@ -3385,8 +3968,11 @@
       <c r="C193" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D193" s="1">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" s="1">
         <v>3518140008</v>
       </c>
@@ -3396,8 +3982,11 @@
       <c r="C194" s="1" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D194" s="1">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" s="1">
         <v>3518140009</v>
       </c>
@@ -3407,8 +3996,11 @@
       <c r="C195" s="1" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D195" s="1">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" s="1">
         <v>3518140010</v>
       </c>
@@ -3418,8 +4010,11 @@
       <c r="C196" s="1" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D196" s="1">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" s="1">
         <v>3518140011</v>
       </c>
@@ -3429,8 +4024,11 @@
       <c r="C197" s="1" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D197" s="1">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" s="1">
         <v>3518140012</v>
       </c>
@@ -3440,8 +4038,11 @@
       <c r="C198" s="1" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D198" s="1">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" s="1">
         <v>3518140013</v>
       </c>
@@ -3451,8 +4052,11 @@
       <c r="C199" s="1" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D199" s="1">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" s="1">
         <v>3518140014</v>
       </c>
@@ -3462,8 +4066,11 @@
       <c r="C200" s="1" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D200" s="1">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" s="1">
         <v>3518140015</v>
       </c>
@@ -3473,8 +4080,11 @@
       <c r="C201" s="1" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D201" s="1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" s="1">
         <v>3518150001</v>
       </c>
@@ -3484,8 +4094,11 @@
       <c r="C202" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D202" s="1">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" s="1">
         <v>3518150002</v>
       </c>
@@ -3495,8 +4108,11 @@
       <c r="C203" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D203" s="1">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" s="1">
         <v>3518150003</v>
       </c>
@@ -3506,8 +4122,11 @@
       <c r="C204" s="1" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D204" s="1">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" s="1">
         <v>3518150004</v>
       </c>
@@ -3517,8 +4136,11 @@
       <c r="C205" s="1" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D205" s="1">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" s="1">
         <v>3518150005</v>
       </c>
@@ -3528,8 +4150,11 @@
       <c r="C206" s="1" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D206" s="1">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" s="1">
         <v>3518150006</v>
       </c>
@@ -3539,8 +4164,11 @@
       <c r="C207" s="1" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D207" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" s="1">
         <v>3518150007</v>
       </c>
@@ -3550,8 +4178,11 @@
       <c r="C208" s="1" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D208" s="1">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" s="1">
         <v>3518150008</v>
       </c>
@@ -3561,8 +4192,11 @@
       <c r="C209" s="1" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D209" s="1">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" s="1">
         <v>3518150009</v>
       </c>
@@ -3572,8 +4206,11 @@
       <c r="C210" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D210" s="1">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" s="1">
         <v>3518150010</v>
       </c>
@@ -3583,8 +4220,11 @@
       <c r="C211" s="1" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D211" s="1">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" s="1">
         <v>3518150011</v>
       </c>
@@ -3594,8 +4234,11 @@
       <c r="C212" s="1" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D212" s="1">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" s="1">
         <v>3518150012</v>
       </c>
@@ -3605,8 +4248,11 @@
       <c r="C213" s="1" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D213" s="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" s="1">
         <v>3518150013</v>
       </c>
@@ -3616,8 +4262,11 @@
       <c r="C214" s="1" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D214" s="1">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" s="1">
         <v>3518150014</v>
       </c>
@@ -3627,8 +4276,11 @@
       <c r="C215" s="1" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D215" s="1">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" s="1">
         <v>3518150015</v>
       </c>
@@ -3638,8 +4290,11 @@
       <c r="C216" s="1" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D216" s="1">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" s="1">
         <v>3518150016</v>
       </c>
@@ -3649,8 +4304,11 @@
       <c r="C217" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D217" s="1">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" s="1">
         <v>3518150017</v>
       </c>
@@ -3660,8 +4318,11 @@
       <c r="C218" s="1" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D218" s="1">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" s="1">
         <v>3518150018</v>
       </c>
@@ -3671,8 +4332,11 @@
       <c r="C219" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D219" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" s="1">
         <v>3518150019</v>
       </c>
@@ -3682,8 +4346,11 @@
       <c r="C220" s="1" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D220" s="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" s="1">
         <v>3518150020</v>
       </c>
@@ -3693,8 +4360,11 @@
       <c r="C221" s="1" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D221" s="1">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" s="1">
         <v>3518150021</v>
       </c>
@@ -3704,8 +4374,11 @@
       <c r="C222" s="1" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D222" s="1">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" s="1">
         <v>3518160001</v>
       </c>
@@ -3715,8 +4388,11 @@
       <c r="C223" s="1" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D223" s="1">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" s="1">
         <v>3518160002</v>
       </c>
@@ -3726,8 +4402,11 @@
       <c r="C224" s="1" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D224" s="1">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" s="1">
         <v>3518160003</v>
       </c>
@@ -3737,8 +4416,11 @@
       <c r="C225" s="1" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D225" s="1">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" s="1">
         <v>3518160004</v>
       </c>
@@ -3748,8 +4430,11 @@
       <c r="C226" s="1" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D226" s="1">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" s="1">
         <v>3518160005</v>
       </c>
@@ -3759,8 +4444,11 @@
       <c r="C227" s="1" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D227" s="1">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" s="1">
         <v>3518160006</v>
       </c>
@@ -3770,8 +4458,11 @@
       <c r="C228" s="1" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D228" s="1">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" s="1">
         <v>3518170001</v>
       </c>
@@ -3781,8 +4472,11 @@
       <c r="C229" s="1" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D229" s="1">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" s="1">
         <v>3518170002</v>
       </c>
@@ -3792,8 +4486,11 @@
       <c r="C230" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D230" s="1">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" s="1">
         <v>3518170003</v>
       </c>
@@ -3803,8 +4500,11 @@
       <c r="C231" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D231" s="1">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" s="1">
         <v>3518170004</v>
       </c>
@@ -3814,8 +4514,11 @@
       <c r="C232" s="1" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D232" s="1">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233" s="1">
         <v>3518170005</v>
       </c>
@@ -3825,8 +4528,11 @@
       <c r="C233" s="1" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D233" s="1">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234" s="1">
         <v>3518170006</v>
       </c>
@@ -3836,8 +4542,11 @@
       <c r="C234" s="1" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D234" s="1">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235" s="1">
         <v>3518170007</v>
       </c>
@@ -3847,8 +4556,11 @@
       <c r="C235" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D235" s="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A236" s="1">
         <v>3518170008</v>
       </c>
@@ -3858,8 +4570,11 @@
       <c r="C236" s="1" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D236" s="1">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A237" s="1">
         <v>3518170009</v>
       </c>
@@ -3869,8 +4584,11 @@
       <c r="C237" s="1" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D237" s="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A238" s="1">
         <v>3518170010</v>
       </c>
@@ -3880,8 +4598,11 @@
       <c r="C238" s="1" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D238" s="1">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A239" s="1">
         <v>3518170011</v>
       </c>
@@ -3891,8 +4612,11 @@
       <c r="C239" s="1" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D239" s="1">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A240" s="1">
         <v>3518170012</v>
       </c>
@@ -3902,8 +4626,11 @@
       <c r="C240" s="1" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D240" s="1">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A241" s="1">
         <v>3518170013</v>
       </c>
@@ -3913,8 +4640,11 @@
       <c r="C241" s="1" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D241" s="1">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A242" s="1">
         <v>3518170014</v>
       </c>
@@ -3924,8 +4654,11 @@
       <c r="C242" s="1" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D242" s="1">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A243" s="1">
         <v>3518170015</v>
       </c>
@@ -3935,8 +4668,11 @@
       <c r="C243" s="1" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D243" s="1">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A244" s="1">
         <v>3518170016</v>
       </c>
@@ -3946,8 +4682,11 @@
       <c r="C244" s="1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D244" s="1">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A245" s="1">
         <v>3518170017</v>
       </c>
@@ -3957,8 +4696,11 @@
       <c r="C245" s="1" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D245" s="1">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A246" s="1">
         <v>3518170018</v>
       </c>
@@ -3968,8 +4710,11 @@
       <c r="C246" s="1" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D246" s="1">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A247" s="1">
         <v>3518170019</v>
       </c>
@@ -3979,8 +4724,11 @@
       <c r="C247" s="1" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D247" s="1">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A248" s="1">
         <v>3518170020</v>
       </c>
@@ -3990,8 +4738,11 @@
       <c r="C248" s="1" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D248" s="1">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A249" s="1">
         <v>3518170021</v>
       </c>
@@ -4001,8 +4752,11 @@
       <c r="C249" s="1" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D249" s="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A250" s="1">
         <v>3518170022</v>
       </c>
@@ -4012,8 +4766,11 @@
       <c r="C250" s="1" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D250" s="1">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A251" s="1">
         <v>3518170023</v>
       </c>
@@ -4023,8 +4780,11 @@
       <c r="C251" s="1" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D251" s="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A252" s="1">
         <v>3518170024</v>
       </c>
@@ -4034,8 +4794,11 @@
       <c r="C252" s="1" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D252" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A253" s="1">
         <v>3518180001</v>
       </c>
@@ -4045,8 +4808,11 @@
       <c r="C253" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D253" s="1">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A254" s="1">
         <v>3518180002</v>
       </c>
@@ -4056,8 +4822,11 @@
       <c r="C254" s="1" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D254" s="1">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A255" s="1">
         <v>3518180003</v>
       </c>
@@ -4067,8 +4836,11 @@
       <c r="C255" s="1" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D255" s="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A256" s="1">
         <v>3518180004</v>
       </c>
@@ -4078,8 +4850,11 @@
       <c r="C256" s="1" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D256" s="1">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A257" s="1">
         <v>3518180005</v>
       </c>
@@ -4089,8 +4864,11 @@
       <c r="C257" s="1" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D257" s="1">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A258" s="1">
         <v>3518180006</v>
       </c>
@@ -4100,8 +4878,11 @@
       <c r="C258" s="1" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D258" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A259" s="1">
         <v>3518190001</v>
       </c>
@@ -4111,8 +4892,11 @@
       <c r="C259" s="1" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D259" s="1">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A260" s="1">
         <v>3518190002</v>
       </c>
@@ -4122,8 +4906,11 @@
       <c r="C260" s="1" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D260" s="1">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A261" s="1">
         <v>3518190003</v>
       </c>
@@ -4133,8 +4920,11 @@
       <c r="C261" s="1" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D261" s="1">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A262" s="1">
         <v>3518190004</v>
       </c>
@@ -4144,8 +4934,11 @@
       <c r="C262" s="1" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D262" s="1">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A263" s="1">
         <v>3518190005</v>
       </c>
@@ -4155,8 +4948,11 @@
       <c r="C263" s="1" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D263" s="1">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A264" s="1">
         <v>3518190006</v>
       </c>
@@ -4166,8 +4962,11 @@
       <c r="C264" s="1" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D264" s="1">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A265" s="1">
         <v>3518190007</v>
       </c>
@@ -4177,8 +4976,11 @@
       <c r="C265" s="1" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D265" s="1">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A266" s="1">
         <v>3518190008</v>
       </c>
@@ -4188,8 +4990,11 @@
       <c r="C266" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D266" s="1">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A267" s="1">
         <v>3518190009</v>
       </c>
@@ -4199,8 +5004,11 @@
       <c r="C267" s="1" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D267" s="1">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A268" s="1">
         <v>3518190010</v>
       </c>
@@ -4210,8 +5018,11 @@
       <c r="C268" s="1" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D268" s="1">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A269" s="1">
         <v>3518190011</v>
       </c>
@@ -4221,8 +5032,11 @@
       <c r="C269" s="1" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D269" s="1">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A270" s="1">
         <v>3518190012</v>
       </c>
@@ -4232,8 +5046,11 @@
       <c r="C270" s="1" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D270" s="1">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A271" s="1">
         <v>3518190013</v>
       </c>
@@ -4243,8 +5060,11 @@
       <c r="C271" s="1" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D271" s="1">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A272" s="1">
         <v>3518190014</v>
       </c>
@@ -4254,8 +5074,11 @@
       <c r="C272" s="1" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D272" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A273" s="1">
         <v>3518190015</v>
       </c>
@@ -4265,8 +5088,11 @@
       <c r="C273" s="1" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D273" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A274" s="1">
         <v>3518190016</v>
       </c>
@@ -4276,8 +5102,11 @@
       <c r="C274" s="1" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D274" s="1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A275" s="1">
         <v>3518200001</v>
       </c>
@@ -4287,8 +5116,11 @@
       <c r="C275" s="1" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D275" s="1">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A276" s="1">
         <v>3518200002</v>
       </c>
@@ -4298,8 +5130,11 @@
       <c r="C276" s="1" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D276" s="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A277" s="1">
         <v>3518200003</v>
       </c>
@@ -4309,8 +5144,11 @@
       <c r="C277" s="1" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D277" s="1">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A278" s="1">
         <v>3518200004</v>
       </c>
@@ -4320,8 +5158,11 @@
       <c r="C278" s="1" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D278" s="1">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A279" s="1">
         <v>3518200005</v>
       </c>
@@ -4331,8 +5172,11 @@
       <c r="C279" s="1" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D279" s="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A280" s="1">
         <v>3518200006</v>
       </c>
@@ -4342,8 +5186,11 @@
       <c r="C280" s="1" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D280" s="1">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A281" s="1">
         <v>3518200007</v>
       </c>
@@ -4353,8 +5200,11 @@
       <c r="C281" s="1" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D281" s="1">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A282" s="1">
         <v>3518200008</v>
       </c>
@@ -4364,8 +5214,11 @@
       <c r="C282" s="1" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D282" s="1">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A283" s="1">
         <v>3518200009</v>
       </c>
@@ -4375,8 +5228,11 @@
       <c r="C283" s="1" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D283" s="1">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A284" s="1">
         <v>3518200010</v>
       </c>
@@ -4386,8 +5242,11 @@
       <c r="C284" s="1" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D284" s="1">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A285" s="1">
         <v>3518200011</v>
       </c>
@@ -4396,6 +5255,9 @@
       </c>
       <c r="C285" s="1" t="s">
         <v>275</v>
+      </c>
+      <c r="D285" s="1">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>